<commit_message>
ControllerFactory zusammengebastelt 80 millionen stunden lang fehler gesucht
</commit_message>
<xml_diff>
--- a/documentation/diagrams/layout.xlsx
+++ b/documentation/diagrams/layout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36eb05c4c24fd3aa/Dokumente/FH/BIF/2023_SS/SWEN2/swen2-project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36eb05c4c24fd3aa/Dokumente/FH/BIF/2023_SS/SWEN2/swen2-project/documentation/diagrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="50" documentId="8_{5B3CD8C0-D586-4DF4-A000-F7DB0D44913F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8803FBB-8D6A-421B-B4A9-C3F01F4FFE68}"/>
@@ -668,7 +668,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>